<commit_message>
add libriaries to requirements
</commit_message>
<xml_diff>
--- a/avans.xlsx
+++ b/avans.xlsx
@@ -31,52 +31,52 @@
     <t>пупкин ИВан</t>
   </si>
   <si>
+    <t>416.67</t>
+  </si>
+  <si>
+    <t>250.0</t>
+  </si>
+  <si>
+    <t>166.67</t>
+  </si>
+  <si>
     <t>Киркоров Филип</t>
   </si>
   <si>
+    <t>982.14</t>
+  </si>
+  <si>
+    <t>150.0</t>
+  </si>
+  <si>
+    <t>832.14</t>
+  </si>
+  <si>
     <t>ww wwww</t>
   </si>
   <si>
+    <t>904.76</t>
+  </si>
+  <si>
+    <t>100.0</t>
+  </si>
+  <si>
+    <t>804.76</t>
+  </si>
+  <si>
     <t>чел Проверочный</t>
   </si>
   <si>
+    <t>0.00</t>
+  </si>
+  <si>
+    <t>-100.00</t>
+  </si>
+  <si>
     <t>один Еще</t>
   </si>
   <si>
-    <t>416.67</t>
-  </si>
-  <si>
-    <t>982.14</t>
-  </si>
-  <si>
-    <t>904.76</t>
-  </si>
-  <si>
-    <t>0.00</t>
-  </si>
-  <si>
     <t>52.38</t>
-  </si>
-  <si>
-    <t>250.0</t>
-  </si>
-  <si>
-    <t>150.0</t>
-  </si>
-  <si>
-    <t>100.0</t>
-  </si>
-  <si>
-    <t>166.67</t>
-  </si>
-  <si>
-    <t>832.14</t>
-  </si>
-  <si>
-    <t>804.76</t>
-  </si>
-  <si>
-    <t>-100.00</t>
   </si>
   <si>
     <t>-47.62</t>
@@ -111,27 +111,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -140,9 +125,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,66 +445,66 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
         <v>21</v>

</xml_diff>